<commit_message>
Added sliders for character sheet
</commit_message>
<xml_diff>
--- a/miracuse_data.xlsx
+++ b/miracuse_data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2058" uniqueCount="826">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2058" uniqueCount="828">
   <si>
     <t xml:space="preserve">Class</t>
   </si>
@@ -298,25 +298,25 @@
     <t xml:space="preserve">Bravo’s Charm</t>
   </si>
   <si>
-    <t xml:space="preserve">An alchemical perfume that draws attention. Can be used to lure monsters, create distractions, and draw the focus of crowds. You have Advantage when making yourself standout, and when flirting.</t>
+    <t xml:space="preserve">An alchemical perfume that draws attention. Can be used to lure monsters, create distractions, and draw the focus of crowds. You have Advantage when making yourself standout, when rallying others, and when flirting.</t>
   </si>
   <si>
     <t xml:space="preserve">Cutting Wit</t>
   </si>
   <si>
-    <t xml:space="preserve">A slender rapier meant for duelling. Using this weapon, you can choose between dealing Physical or Mental damage. You have Advantage when provoking others.</t>
+    <t xml:space="preserve">A slender rapier meant for duelling. Using this weapon, you can choose between dealing Physical or Mental damage. You have Advantage when intimidating or provoking others.</t>
   </si>
   <si>
     <t xml:space="preserve">Honeyed Words</t>
   </si>
   <si>
-    <t xml:space="preserve">A handful of alchemic candies that diminish pain and induce sleep. Can be used to endure harm, tranquilize unwary guards, and ease suffering. You have Advantage on rolls to resist discomfort or pain.</t>
+    <t xml:space="preserve">A handful of alchemic candies that diminish pain and induce sleep. Can be used to endure harm, tranquilize unwary guards, and ease suffering. You have Advantage on rolls to resist discomfort, or when bribing others.</t>
   </si>
   <si>
     <t xml:space="preserve">Lover’s Embrace</t>
   </si>
   <si>
-    <t xml:space="preserve">Charmed cloth that can change its properties on command. Can be extended into a length of sturdy rope, used as a whip, and made rigid as steel. Often worn as a scarf or other accessory. You have Advantage when climbing.</t>
+    <t xml:space="preserve">A charmed scarf that can change its properties on command. Can be extended into a length of sturdy rope, used as a whip, or made rigid as steel. You have Advantage when interrogating someone restrained by this kit.</t>
   </si>
   <si>
     <t xml:space="preserve">Sharp Retort</t>
@@ -325,7 +325,25 @@
     <t xml:space="preserve">Gear, Weapon, Defense, Reaction</t>
   </si>
   <si>
-    <t xml:space="preserve">A long dagger held in the off-hand, intended to parry and riposte. Using this weapon to attack gives you Advantage on rolls to defend until the start of your next turn. On a successful defense against a melee attack, the attacker takes a box of Physical damage.</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">A long dagger held in the off-hand, intended to parry and riposte. Using this weapon to attack gives you Advantage on rolls to defend until the start of your next turn. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">On a successful defense against a melee attack, you inflict a box of Physical damage to the attacker. </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Venomous Smile</t>
@@ -683,7 +701,7 @@
     <t xml:space="preserve">Warded Greatcoat</t>
   </si>
   <si>
-    <t xml:space="preserve">A leather jacket that reaches past the knees. Sigils of protection have been stitched into the lining, making the wearer resistant to bullets and blunt trauma. You have Advantage when defending against bludgeoning.</t>
+    <t xml:space="preserve">A leather jacket imbued with protective magic. You have Advantage when defending against bludgeoning, such as bullets or clubs.</t>
   </si>
   <si>
     <t xml:space="preserve">Knight</t>
@@ -1031,7 +1049,7 @@
     <t xml:space="preserve">Flying Broom</t>
   </si>
   <si>
-    <t xml:space="preserve">An enchanted staff built using the same principles as airships. Can be used to fly through the air with ease.</t>
+    <t xml:space="preserve">An enchanted staff built using the same principles as airships. Can be used to fly through the air with ease and at high speeds. You have Advantage when dodging attacks while on the broom.</t>
   </si>
   <si>
     <t xml:space="preserve">Slowing Thorns</t>
@@ -1554,6 +1572,9 @@
   </si>
   <si>
     <t xml:space="preserve">Gladiator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A slender rapier meant for duelling. Using this weapon, you can choose between dealing Physical or Mental damage. You have Advantage when provoking others.</t>
   </si>
   <si>
     <r>
@@ -1575,6 +1596,9 @@
       </rPr>
       <t xml:space="preserve">Using this weapon to attack gives you Advantage on rolls to defend until the start of your next turn. On a successful defense against a melee attack, the attacker takes a box of Physical damage.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">An alchemical perfume that draws attention. Can be used to lure monsters, create distractions, and draw the focus of crowds. You have Advantage when making yourself standout, and when flirting.</t>
   </si>
   <si>
     <t xml:space="preserve">A handful of alchemic candies that diminish pain and induce sleep. Can be used to endure harm, tranquilize unwary guards, and ease suffering. You have Advantage on rolls to resist discomfort.</t>
@@ -3331,8 +3355,8 @@
   </sheetPr>
   <dimension ref="A1:E145"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C109" activeCellId="0" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5622,7 +5646,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="4" t="s">
         <v>5</v>
       </c>
@@ -5633,7 +5657,7 @@
         <v>321</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="E135" s="7" t="s">
         <v>322</v>
@@ -7368,7 +7392,7 @@
         <v>62</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>89</v>
+        <v>497</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="51.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7385,7 +7409,7 @@
         <v>95</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7402,7 +7426,7 @@
         <v>25</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>87</v>
+        <v>499</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7436,7 +7460,7 @@
         <v>25</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7453,7 +7477,7 @@
         <v>17</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7503,7 +7527,7 @@
         <v>5</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C92" s="6"/>
       <c r="D92" s="6"/>
@@ -7514,7 +7538,7 @@
         <v>5</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C93" s="6"/>
       <c r="D93" s="6"/>
@@ -7525,7 +7549,7 @@
         <v>5</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
@@ -7536,7 +7560,7 @@
         <v>5</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
@@ -7547,7 +7571,7 @@
         <v>5</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C96" s="6"/>
       <c r="D96" s="6"/>
@@ -7558,7 +7582,7 @@
         <v>5</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C97" s="6"/>
       <c r="D97" s="6"/>
@@ -7569,16 +7593,16 @@
         <v>5</v>
       </c>
       <c r="B98" s="21" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="C98" s="22" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="D98" s="22" t="s">
         <v>38</v>
       </c>
       <c r="E98" s="23" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="51.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7586,16 +7610,16 @@
         <v>5</v>
       </c>
       <c r="B99" s="21" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="C99" s="22" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="D99" s="22" t="s">
         <v>38</v>
       </c>
       <c r="E99" s="23" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7603,16 +7627,16 @@
         <v>5</v>
       </c>
       <c r="B100" s="21" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="C100" s="22" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="D100" s="22" t="s">
         <v>38</v>
       </c>
       <c r="E100" s="23" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7620,16 +7644,16 @@
         <v>5</v>
       </c>
       <c r="B101" s="21" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="C101" s="22" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="D101" s="22" t="s">
         <v>25</v>
       </c>
       <c r="E101" s="23" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7637,10 +7661,10 @@
         <v>5</v>
       </c>
       <c r="B102" s="21" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="C102" s="22" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="D102" s="22" t="s">
         <v>25</v>
@@ -7652,7 +7676,7 @@
         <v>5</v>
       </c>
       <c r="B103" s="21" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="C103" s="22"/>
       <c r="D103" s="22"/>
@@ -7764,13 +7788,13 @@
         <v>264</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7779,13 +7803,13 @@
         <v>264</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>409</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7814,16 +7838,16 @@
         <v>70</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7831,16 +7855,16 @@
         <v>70</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7848,16 +7872,16 @@
         <v>70</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7865,16 +7889,16 @@
         <v>70</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7882,16 +7906,16 @@
         <v>70</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7899,68 +7923,68 @@
         <v>70</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="16"/>
       <c r="B13" s="17"/>
       <c r="C13" s="18" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="16"/>
       <c r="B14" s="17"/>
       <c r="C14" s="18" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="16"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="16"/>
       <c r="B16" s="17"/>
       <c r="C16" s="18" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7998,7 +8022,7 @@
         <v>38</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8015,7 +8039,7 @@
         <v>38</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8032,7 +8056,7 @@
         <v>38</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8043,13 +8067,13 @@
         <v>278</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>38</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8066,7 +8090,7 @@
         <v>38</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8083,7 +8107,7 @@
         <v>38</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8301,16 +8325,16 @@
         <v>54</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="D56" s="14" t="s">
         <v>409</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8318,16 +8342,16 @@
         <v>54</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="D57" s="14" t="s">
         <v>409</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8363,16 +8387,16 @@
         <v>54</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>222</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8380,16 +8404,16 @@
         <v>54</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C63" s="14" t="s">
         <v>152</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8397,16 +8421,16 @@
         <v>54</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="D64" s="14" t="s">
         <v>25</v>
       </c>
       <c r="E64" s="15" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8414,16 +8438,16 @@
         <v>54</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C65" s="14" t="s">
         <v>228</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8431,16 +8455,16 @@
         <v>54</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C66" s="14" t="s">
         <v>132</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="E66" s="15" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8448,13 +8472,13 @@
         <v>54</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C67" s="14" t="s">
         <v>232</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="E67" s="15" t="s">
         <v>234</v>
@@ -8471,13 +8495,13 @@
       <c r="A69" s="12"/>
       <c r="B69" s="13"/>
       <c r="C69" s="14" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="E69" s="15" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8487,23 +8511,23 @@
         <v>169</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="E70" s="15" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="12"/>
       <c r="B71" s="13"/>
       <c r="C71" s="14" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="D71" s="14" t="s">
         <v>25</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8528,13 +8552,13 @@
         <v>193</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="68" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8548,10 +8572,10 @@
         <v>199</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8562,13 +8586,13 @@
         <v>193</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="68" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8579,13 +8603,13 @@
         <v>193</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="68" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8602,7 +8626,7 @@
         <v>25</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="84.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8613,13 +8637,13 @@
         <v>193</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="68" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -8716,13 +8740,13 @@
         <v>71</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>409</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8733,13 +8757,13 @@
         <v>71</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8756,7 +8780,7 @@
         <v>25</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8767,13 +8791,13 @@
         <v>71</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8790,7 +8814,7 @@
         <v>25</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8801,13 +8825,13 @@
         <v>71</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8824,7 +8848,7 @@
         <v>25</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8835,13 +8859,13 @@
         <v>151</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>156</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8858,7 +8882,7 @@
         <v>25</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8869,13 +8893,13 @@
         <v>151</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8886,13 +8910,13 @@
         <v>151</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8903,13 +8927,13 @@
         <v>151</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8920,13 +8944,13 @@
         <v>264</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>409</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8937,13 +8961,13 @@
         <v>264</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8954,13 +8978,13 @@
         <v>264</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8971,13 +8995,13 @@
         <v>264</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8994,7 +9018,7 @@
         <v>25</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9005,13 +9029,13 @@
         <v>264</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9022,13 +9046,13 @@
         <v>236</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>475</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9039,13 +9063,13 @@
         <v>236</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="D21" s="26" t="s">
         <v>448</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9056,13 +9080,13 @@
         <v>236</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>448</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9073,13 +9097,13 @@
         <v>236</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>448</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9090,13 +9114,13 @@
         <v>236</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="D24" s="26" t="s">
         <v>448</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9107,13 +9131,13 @@
         <v>236</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="D25" s="26" t="s">
         <v>448</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9124,13 +9148,13 @@
         <v>278</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="D26" s="26" t="s">
         <v>448</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9141,13 +9165,13 @@
         <v>278</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="D27" s="26" t="s">
         <v>448</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9158,13 +9182,13 @@
         <v>278</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="D28" s="26" t="s">
         <v>448</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9175,13 +9199,13 @@
         <v>278</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="D29" s="26" t="s">
         <v>448</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9192,13 +9216,13 @@
         <v>278</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="D30" s="26" t="s">
         <v>448</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9209,13 +9233,13 @@
         <v>278</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="D31" s="26" t="s">
         <v>448</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9226,13 +9250,13 @@
         <v>331</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="D32" s="26" t="s">
         <v>419</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9243,13 +9267,13 @@
         <v>331</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="D33" s="26" t="s">
         <v>448</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9260,13 +9284,13 @@
         <v>331</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="D34" s="26" t="s">
         <v>475</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9277,13 +9301,13 @@
         <v>331</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="D35" s="26" t="s">
         <v>448</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9294,13 +9318,13 @@
         <v>331</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="D36" s="26" t="s">
         <v>448</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9311,13 +9335,13 @@
         <v>331</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="D37" s="26" t="s">
         <v>448</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9334,7 +9358,7 @@
         <v>25</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9351,7 +9375,7 @@
         <v>25</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9362,13 +9386,13 @@
         <v>23</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>409</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9379,13 +9403,13 @@
         <v>23</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>409</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9396,13 +9420,13 @@
         <v>23</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9413,13 +9437,13 @@
         <v>23</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="D43" s="10" t="s">
         <v>448</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9430,13 +9454,13 @@
         <v>40</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>409</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9453,7 +9477,7 @@
         <v>25</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9470,7 +9494,7 @@
         <v>156</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9481,13 +9505,13 @@
         <v>40</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="D47" s="10" t="s">
         <v>448</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9498,13 +9522,13 @@
         <v>40</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="D48" s="10" t="s">
         <v>448</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9515,13 +9539,13 @@
         <v>40</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="D49" s="10" t="s">
         <v>419</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9532,13 +9556,13 @@
         <v>250</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="D50" s="10" t="s">
         <v>409</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9549,13 +9573,13 @@
         <v>250</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="D51" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9566,13 +9590,13 @@
         <v>250</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="D52" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9583,13 +9607,13 @@
         <v>250</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="D53" s="10" t="s">
         <v>419</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9600,13 +9624,13 @@
         <v>250</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="D54" s="10" t="s">
         <v>409</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9617,13 +9641,13 @@
         <v>250</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="D55" s="10" t="s">
         <v>448</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9631,16 +9655,16 @@
         <v>54</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="D56" s="14" t="s">
         <v>409</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9648,16 +9672,16 @@
         <v>54</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="D57" s="14" t="s">
         <v>419</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9665,16 +9689,16 @@
         <v>54</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="D58" s="14" t="s">
         <v>409</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9682,16 +9706,16 @@
         <v>54</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="D59" s="14" t="s">
         <v>409</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9699,16 +9723,16 @@
         <v>54</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9716,7 +9740,7 @@
         <v>54</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C61" s="14" t="s">
         <v>66</v>
@@ -9725,7 +9749,7 @@
         <v>409</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9736,13 +9760,13 @@
         <v>207</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="D62" s="14" t="s">
         <v>466</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9759,7 +9783,7 @@
         <v>25</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9770,13 +9794,13 @@
         <v>207</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="D64" s="14" t="s">
         <v>409</v>
       </c>
       <c r="E64" s="15" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9787,13 +9811,13 @@
         <v>207</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="D65" s="14" t="s">
         <v>419</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9804,13 +9828,13 @@
         <v>207</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="D66" s="14" t="s">
         <v>409</v>
       </c>
       <c r="E66" s="15" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9821,13 +9845,13 @@
         <v>207</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="D67" s="14" t="s">
         <v>409</v>
       </c>
       <c r="E67" s="15" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9835,16 +9859,16 @@
         <v>54</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="E68" s="15" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9852,16 +9876,16 @@
         <v>54</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="D69" s="14" t="s">
         <v>409</v>
       </c>
       <c r="E69" s="15" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9869,16 +9893,16 @@
         <v>54</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="D70" s="14" t="s">
         <v>419</v>
       </c>
       <c r="E70" s="15" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9886,16 +9910,16 @@
         <v>54</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="D71" s="14" t="s">
         <v>466</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9903,16 +9927,16 @@
         <v>54</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="D72" s="14" t="s">
         <v>409</v>
       </c>
       <c r="E72" s="15" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9920,16 +9944,16 @@
         <v>54</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="D73" s="14" t="s">
         <v>466</v>
       </c>
       <c r="E73" s="15" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="68" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -10032,13 +10056,13 @@
         <v>71</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10052,10 +10076,10 @@
         <v>43</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10069,10 +10093,10 @@
         <v>24</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10086,10 +10110,10 @@
         <v>48</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10103,10 +10127,10 @@
         <v>33</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10117,13 +10141,13 @@
         <v>71</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10134,13 +10158,13 @@
         <v>151</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10151,13 +10175,13 @@
         <v>151</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10168,13 +10192,13 @@
         <v>151</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10185,13 +10209,13 @@
         <v>151</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10202,13 +10226,13 @@
         <v>151</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10219,13 +10243,13 @@
         <v>151</v>
       </c>
       <c r="C13" s="18" t="s">
+        <v>723</v>
+      </c>
+      <c r="D13" s="18" t="s">
         <v>721</v>
       </c>
-      <c r="D13" s="18" t="s">
-        <v>719</v>
-      </c>
       <c r="E13" s="19" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10239,10 +10263,10 @@
         <v>265</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10253,13 +10277,13 @@
         <v>264</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10270,13 +10294,13 @@
         <v>264</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10287,13 +10311,13 @@
         <v>264</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10307,10 +10331,10 @@
         <v>276</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10321,13 +10345,13 @@
         <v>264</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10338,13 +10362,13 @@
         <v>236</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10355,13 +10379,13 @@
         <v>236</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10372,13 +10396,13 @@
         <v>236</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10389,13 +10413,13 @@
         <v>236</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10406,13 +10430,13 @@
         <v>236</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10423,13 +10447,13 @@
         <v>236</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10440,13 +10464,13 @@
         <v>278</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10457,13 +10481,13 @@
         <v>278</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10474,13 +10498,13 @@
         <v>278</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10491,13 +10515,13 @@
         <v>278</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10508,13 +10532,13 @@
         <v>278</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10525,13 +10549,13 @@
         <v>278</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10542,13 +10566,13 @@
         <v>331</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10559,13 +10583,13 @@
         <v>331</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10576,13 +10600,13 @@
         <v>331</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10593,13 +10617,13 @@
         <v>331</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10610,13 +10634,13 @@
         <v>331</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10627,13 +10651,13 @@
         <v>331</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10644,13 +10668,13 @@
         <v>23</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10661,13 +10685,13 @@
         <v>23</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10678,13 +10702,13 @@
         <v>23</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10695,13 +10719,13 @@
         <v>23</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10712,13 +10736,13 @@
         <v>23</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10729,13 +10753,13 @@
         <v>23</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10746,13 +10770,13 @@
         <v>40</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10763,13 +10787,13 @@
         <v>40</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10780,13 +10804,13 @@
         <v>40</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10797,13 +10821,13 @@
         <v>40</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10814,13 +10838,13 @@
         <v>40</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10831,13 +10855,13 @@
         <v>40</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10848,13 +10872,13 @@
         <v>250</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10865,13 +10889,13 @@
         <v>250</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10882,13 +10906,13 @@
         <v>250</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10899,13 +10923,13 @@
         <v>250</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10916,13 +10940,13 @@
         <v>250</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10933,13 +10957,13 @@
         <v>250</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10947,16 +10971,16 @@
         <v>54</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10964,16 +10988,16 @@
         <v>54</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10981,16 +11005,16 @@
         <v>54</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10998,16 +11022,16 @@
         <v>54</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11015,16 +11039,16 @@
         <v>54</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11032,16 +11056,16 @@
         <v>54</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11052,13 +11076,13 @@
         <v>207</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11069,13 +11093,13 @@
         <v>207</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11086,13 +11110,13 @@
         <v>207</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="E64" s="15" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11103,13 +11127,13 @@
         <v>207</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11120,13 +11144,13 @@
         <v>207</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="E66" s="15" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11137,13 +11161,13 @@
         <v>207</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="E67" s="15" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11151,16 +11175,16 @@
         <v>54</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="E68" s="15" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11168,16 +11192,16 @@
         <v>54</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="E69" s="15" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11185,16 +11209,16 @@
         <v>54</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="E70" s="15" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11202,16 +11226,16 @@
         <v>54</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11219,16 +11243,16 @@
         <v>54</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="E72" s="15" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11236,16 +11260,16 @@
         <v>54</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="E73" s="15" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="68" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Styling for resource boxes
</commit_message>
<xml_diff>
--- a/miracuse_data.xlsx
+++ b/miracuse_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kit" sheetId="1" state="visible" r:id="rId2"/>
@@ -115,25 +115,7 @@
     <t xml:space="preserve">Gear, Weapon, Ranged</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">A set of transparent needles used to deliver poison. Using this weapon allows you to administer poison in the same action as an attack. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">You have Advantage when disguising your sneak attacks to avoid notice.</t>
-    </r>
+    <t xml:space="preserve">A set of transparent needles used to deliver poison. Using this weapon allows you to administer poison in the same action as an attack. You have Advantage when disguising your sneak attacks to avoid notice.</t>
   </si>
   <si>
     <t xml:space="preserve">Golden Silk</t>
@@ -643,25 +625,7 @@
     <t xml:space="preserve">Gear, Weapon, Ranged, Defense</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">A pistol intended for formal duels. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Using this weapon gives you Advantage on rolls to defend against ranged attacks until the start of your next turn. You have Advantage when provoking others.</t>
-    </r>
+    <t xml:space="preserve">A pistol intended for formal duels. Using this weapon gives you Advantage on rolls to defend against ranged attacks until the start of your next turn. You have Advantage when provoking others.</t>
   </si>
   <si>
     <t xml:space="preserve">Magic Bullets</t>
@@ -817,25 +781,7 @@
     <t xml:space="preserve">Talisman of Divination</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">A wand or other object that can be used to petition otherworldly forces for information. Can be used to divine the location of people, places, and things through magical means. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">You have Advantage when identifying magic or magical effects.</t>
-    </r>
+    <t xml:space="preserve">A wand or other object that can be used to petition otherworldly forces for information. Can be used to divine the location of people, places, and things through magical means. You have Advantage when identifying magic or magical effects.</t>
   </si>
   <si>
     <t xml:space="preserve">Talisman of Dreaming</t>
@@ -847,35 +793,7 @@
     <t xml:space="preserve">Talisman of Necromancy</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">A wand or other object that </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">influences</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> the boundary between life and death. Can be used to heal Physical damage, summon ghosts for information, and create undead. The number of Physical boxes healed is equal to the result of the roll.</t>
-    </r>
+    <t xml:space="preserve">A wand or other object that influences the boundary between life and death. Can be used to heal Physical damage, summon ghosts for information, and create undead. The number of Physical boxes healed is equal to the result of the roll.</t>
   </si>
   <si>
     <t xml:space="preserve">Ranger</t>
@@ -1031,25 +949,7 @@
     <t xml:space="preserve">Talisman of Sun</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">A wand or other object that can be used to radiate heat and light from your body. Can be used to burn off restraints, blind nearby enemies, and stave off cold. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">On a successful defense against a melee attack, you inflict a box of Physical damage to the attacker. </t>
-    </r>
+    <t xml:space="preserve">A wand or other object that can be used to radiate heat and light from your body. Can be used to burn off restraints, blind nearby enemies, and stave off cold. On a successful defense against a melee attack, you inflict a box of Physical damage to the attacker. </t>
   </si>
   <si>
     <t xml:space="preserve">Talisman of Terra</t>
@@ -1130,25 +1030,7 @@
     <t xml:space="preserve">Talisman of Restoration</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">A wand or other object that mends that which is broken. Can be used to fix damaged objects, repair enchanted items, and heal wounds. You have Advantage when repairing objects. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">The number of Physical boxes healed is equal to the result of the roll.</t>
-    </r>
+    <t xml:space="preserve">A wand or other object that mends that which is broken. Can be used to fix damaged objects, repair enchanted items, and heal wounds. You have Advantage when repairing objects. The number of Physical boxes healed is equal to the result of the roll.</t>
   </si>
   <si>
     <t xml:space="preserve">Willow Perfume</t>
@@ -1202,13 +1084,13 @@
     <t xml:space="preserve">Perception, Knowledge</t>
   </si>
   <si>
-    <t xml:space="preserve">An adventurer with a keen mind and a watchful eye. Known for their healing potions and skill with firearms.</t>
+    <t xml:space="preserve">An adventurer with a keen mind and a watchful eye. Known for their healing potions and miraculous tools.</t>
   </si>
   <si>
     <t xml:space="preserve">Magic, Presence</t>
   </si>
   <si>
-    <t xml:space="preserve">An adventurer with command over otherworldly forces. Known for their ability to perform magic through talismans.</t>
+    <t xml:space="preserve">An adventurer with command over otherworldly forces. Known for their skill with Talismans.</t>
   </si>
   <si>
     <t xml:space="preserve">Agility, Cunning</t>
@@ -2677,7 +2559,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2737,12 +2619,6 @@
       <name val="Fira Sans"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Fira Sans"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="19">
@@ -3437,9 +3313,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:E145"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -5916,48 +5792,6 @@
       <c r="E145" s="27" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="0"/>
-      <c r="B146" s="0"/>
-      <c r="C146" s="0"/>
-      <c r="D146" s="0"/>
-      <c r="E146" s="0"/>
-    </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="0"/>
-      <c r="B147" s="0"/>
-      <c r="C147" s="0"/>
-      <c r="D147" s="0"/>
-      <c r="E147" s="0"/>
-    </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="0"/>
-      <c r="B148" s="0"/>
-      <c r="C148" s="0"/>
-      <c r="D148" s="0"/>
-      <c r="E148" s="0"/>
-    </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="0"/>
-      <c r="B149" s="0"/>
-      <c r="C149" s="0"/>
-      <c r="D149" s="0"/>
-      <c r="E149" s="0"/>
-    </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="0"/>
-      <c r="B150" s="0"/>
-      <c r="C150" s="0"/>
-      <c r="D150" s="0"/>
-      <c r="E150" s="0"/>
-    </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="0"/>
-      <c r="B151" s="0"/>
-      <c r="C151" s="0"/>
-      <c r="D151" s="0"/>
-      <c r="E151" s="0"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E145"/>
@@ -5979,8 +5813,8 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>